<commit_message>
Creating cells method update
</commit_message>
<xml_diff>
--- a/Exchange rate.xlsx
+++ b/Exchange rate.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
   <si>
     <t>table</t>
   </si>
@@ -35,10 +35,127 @@
     <t>USD</t>
   </si>
   <si>
-    <t>{no=027/A/NBP/2021, effectiveDate=2021-02-10, mid=3.6973}</t>
-  </si>
-  <si>
-    <t>{no=029/A/NBP/2021, effectiveDate=2021-02-12, mid=3.7186}</t>
+    <t>026/A/NBP/2021</t>
+  </si>
+  <si>
+    <t>2021-02-09</t>
+  </si>
+  <si>
+    <t>3.6972</t>
+  </si>
+  <si>
+    <t>027/A/NBP/2021</t>
+  </si>
+  <si>
+    <t>2021-02-10</t>
+  </si>
+  <si>
+    <t>3.6973</t>
+  </si>
+  <si>
+    <t>028/A/NBP/2021</t>
+  </si>
+  <si>
+    <t>2021-02-11</t>
+  </si>
+  <si>
+    <t>3.7117</t>
+  </si>
+  <si>
+    <t>029/A/NBP/2021</t>
+  </si>
+  <si>
+    <t>2021-02-12</t>
+  </si>
+  <si>
+    <t>3.7186</t>
+  </si>
+  <si>
+    <t>030/A/NBP/2021</t>
+  </si>
+  <si>
+    <t>2021-02-15</t>
+  </si>
+  <si>
+    <t>3.6949</t>
+  </si>
+  <si>
+    <t>031/A/NBP/2021</t>
+  </si>
+  <si>
+    <t>2021-02-16</t>
+  </si>
+  <si>
+    <t>3.694</t>
+  </si>
+  <si>
+    <t>032/A/NBP/2021</t>
+  </si>
+  <si>
+    <t>2021-02-17</t>
+  </si>
+  <si>
+    <t>3.7287</t>
+  </si>
+  <si>
+    <t>033/A/NBP/2021</t>
+  </si>
+  <si>
+    <t>2021-02-18</t>
+  </si>
+  <si>
+    <t>3.7152</t>
+  </si>
+  <si>
+    <t>034/A/NBP/2021</t>
+  </si>
+  <si>
+    <t>2021-02-19</t>
+  </si>
+  <si>
+    <t>3.6997</t>
+  </si>
+  <si>
+    <t>035/A/NBP/2021</t>
+  </si>
+  <si>
+    <t>2021-02-22</t>
+  </si>
+  <si>
+    <t>3.7135</t>
+  </si>
+  <si>
+    <t>036/A/NBP/2021</t>
+  </si>
+  <si>
+    <t>2021-02-23</t>
+  </si>
+  <si>
+    <t>037/A/NBP/2021</t>
+  </si>
+  <si>
+    <t>2021-02-24</t>
+  </si>
+  <si>
+    <t>3.7145</t>
+  </si>
+  <si>
+    <t>038/A/NBP/2021</t>
+  </si>
+  <si>
+    <t>2021-02-25</t>
+  </si>
+  <si>
+    <t>3.6943</t>
+  </si>
+  <si>
+    <t>039/A/NBP/2021</t>
+  </si>
+  <si>
+    <t>2021-02-26</t>
+  </si>
+  <si>
+    <t>3.7247</t>
   </si>
 </sst>
 </file>
@@ -83,7 +200,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -113,14 +230,159 @@
       <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="D2"/>
     </row>
     <row r="3">
-      <c r="A3" t="s">
+      <c r="D3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
         <v>8</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="D6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="D7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="D8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="D9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="D10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="D11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="D12" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" t="s">
+        <v>35</v>
+      </c>
+      <c r="F12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="D13" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" t="s">
+        <v>38</v>
+      </c>
+      <c r="F13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="D14" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" t="s">
+        <v>40</v>
+      </c>
+      <c r="F14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="D15" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F15" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="D16" t="s">
+        <v>45</v>
+      </c>
+      <c r="E16" t="s">
+        <v>46</v>
+      </c>
+      <c r="F16" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cells method update. Set in excel file
</commit_message>
<xml_diff>
--- a/Exchange rate.xlsx
+++ b/Exchange rate.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="46">
   <si>
     <t>table</t>
   </si>
@@ -35,6 +35,9 @@
     <t>USD</t>
   </si>
   <si>
+    <t>[no, effectiveDate, mid]</t>
+  </si>
+  <si>
     <t>026/A/NBP/2021</t>
   </si>
   <si>
@@ -69,6 +72,84 @@
   </si>
   <si>
     <t>3.7186</t>
+  </si>
+  <si>
+    <t>030/A/NBP/2021</t>
+  </si>
+  <si>
+    <t>2021-02-15</t>
+  </si>
+  <si>
+    <t>3.6949</t>
+  </si>
+  <si>
+    <t>031/A/NBP/2021</t>
+  </si>
+  <si>
+    <t>2021-02-16</t>
+  </si>
+  <si>
+    <t>3.694</t>
+  </si>
+  <si>
+    <t>032/A/NBP/2021</t>
+  </si>
+  <si>
+    <t>2021-02-17</t>
+  </si>
+  <si>
+    <t>3.7287</t>
+  </si>
+  <si>
+    <t>033/A/NBP/2021</t>
+  </si>
+  <si>
+    <t>2021-02-18</t>
+  </si>
+  <si>
+    <t>3.7152</t>
+  </si>
+  <si>
+    <t>034/A/NBP/2021</t>
+  </si>
+  <si>
+    <t>2021-02-19</t>
+  </si>
+  <si>
+    <t>3.6997</t>
+  </si>
+  <si>
+    <t>035/A/NBP/2021</t>
+  </si>
+  <si>
+    <t>2021-02-22</t>
+  </si>
+  <si>
+    <t>3.7135</t>
+  </si>
+  <si>
+    <t>036/A/NBP/2021</t>
+  </si>
+  <si>
+    <t>2021-02-23</t>
+  </si>
+  <si>
+    <t>037/A/NBP/2021</t>
+  </si>
+  <si>
+    <t>2021-02-24</t>
+  </si>
+  <si>
+    <t>3.7145</t>
+  </si>
+  <si>
+    <t>038/A/NBP/2021</t>
+  </si>
+  <si>
+    <t>2021-02-25</t>
+  </si>
+  <si>
+    <t>3.6943</t>
   </si>
 </sst>
 </file>
@@ -113,7 +194,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -143,49 +224,157 @@
       <c r="C2" t="s">
         <v>6</v>
       </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="3">
       <c r="D3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4">
       <c r="D4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5">
       <c r="D5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6">
       <c r="D6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="D7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="D8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="D9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="D10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="D11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="D12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" t="s">
+        <v>36</v>
+      </c>
+      <c r="F12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="D13" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" t="s">
+        <v>39</v>
+      </c>
+      <c r="F13" t="s">
         <v>16</v>
       </c>
-      <c r="E6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" t="s">
-        <v>18</v>
+    </row>
+    <row r="14">
+      <c r="D14" t="s">
+        <v>40</v>
+      </c>
+      <c r="E14" t="s">
+        <v>41</v>
+      </c>
+      <c r="F14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="D15" t="s">
+        <v>43</v>
+      </c>
+      <c r="E15" t="s">
+        <v>44</v>
+      </c>
+      <c r="F15" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CreateMyCells finally work. Change headers cells style bold=true.
</commit_message>
<xml_diff>
--- a/Exchange rate.xlsx
+++ b/Exchange rate.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
   <si>
     <t>table</t>
   </si>
@@ -35,7 +35,13 @@
     <t>USD</t>
   </si>
   <si>
-    <t>[no, effectiveDate, mid]</t>
+    <t>no</t>
+  </si>
+  <si>
+    <t>effectiveDate</t>
+  </si>
+  <si>
+    <t>mid</t>
   </si>
   <si>
     <t>026/A/NBP/2021</t>
@@ -157,13 +163,18 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
     </font>
   </fonts>
   <fills count="2">
@@ -186,8 +197,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
 </styleSheet>
 </file>
@@ -201,16 +213,16 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="1">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="1">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="1">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="1">
         <v>3</v>
       </c>
     </row>
@@ -228,153 +240,153 @@
         <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3">
       <c r="D3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4">
       <c r="D4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5">
       <c r="D5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6">
       <c r="D6" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E6" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F6" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7">
       <c r="D7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E7" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F7" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8">
       <c r="D8" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E8" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F8" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9">
       <c r="D9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E9" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F9" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10">
       <c r="D10" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E10" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F10" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11">
       <c r="D11" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E11" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F11" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12">
       <c r="D12" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E12" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F12" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13">
       <c r="D13" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E13" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F13" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14">
       <c r="D14" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E14" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F14" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15">
       <c r="D15" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E15" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F15" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Backend finally ready 1.0. Scene Builder and JavaFx configured.
</commit_message>
<xml_diff>
--- a/Exchange rate.xlsx
+++ b/Exchange rate.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="30">
   <si>
     <t>TABLE</t>
   </si>
@@ -45,6 +45,15 @@
     <t>mid</t>
   </si>
   <si>
+    <t>040/A/NBP/2021</t>
+  </si>
+  <si>
+    <t>2021-03-01</t>
+  </si>
+  <si>
+    <t>4.5231</t>
+  </si>
+  <si>
     <t>041/A/NBP/2021</t>
   </si>
   <si>
@@ -54,13 +63,46 @@
     <t>4.5345</t>
   </si>
   <si>
+    <t>042/A/NBP/2021</t>
+  </si>
+  <si>
+    <t>2021-03-03</t>
+  </si>
+  <si>
+    <t>4.5393</t>
+  </si>
+  <si>
+    <t>043/A/NBP/2021</t>
+  </si>
+  <si>
+    <t>2021-03-04</t>
+  </si>
+  <si>
+    <t>4.554</t>
+  </si>
+  <si>
+    <t>044/A/NBP/2021</t>
+  </si>
+  <si>
+    <t>2021-03-05</t>
+  </si>
+  <si>
+    <t>4.5793</t>
+  </si>
+  <si>
     <t>dolar amerykański</t>
   </si>
   <si>
     <t>USD</t>
   </si>
   <si>
+    <t>3.7572</t>
+  </si>
+  <si>
     <t>3.7765</t>
+  </si>
+  <si>
+    <t>3.7509</t>
   </si>
 </sst>
 </file>
@@ -153,7 +195,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -212,6 +254,50 @@
         <v>12</v>
       </c>
     </row>
+    <row r="4">
+      <c r="D4" t="s" s="3">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s" s="3">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s" s="3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="D5" t="s" s="3">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s" s="3">
+        <v>17</v>
+      </c>
+      <c r="F5" t="s" s="3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="D6" t="s" s="3">
+        <v>19</v>
+      </c>
+      <c r="E6" t="s" s="3">
+        <v>20</v>
+      </c>
+      <c r="F6" t="s" s="3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="D7" t="s" s="3">
+        <v>22</v>
+      </c>
+      <c r="E7" t="s" s="3">
+        <v>23</v>
+      </c>
+      <c r="F7" t="s" s="3">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="D1:F1"/>
@@ -222,7 +308,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -255,10 +341,10 @@
         <v>4</v>
       </c>
       <c r="B2" t="s" s="5">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="C2" t="s" s="5">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="D2" t="s" s="5">
         <v>7</v>
@@ -278,7 +364,29 @@
         <v>11</v>
       </c>
       <c r="F3" t="s" s="6">
-        <v>15</v>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="D4" t="s" s="6">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s" s="6">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s" s="6">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="D5" t="s" s="6">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s" s="6">
+        <v>17</v>
+      </c>
+      <c r="F5" t="s" s="6">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Backend finally ready 1.0. Scene Builder and .fxml file config.
</commit_message>
<xml_diff>
--- a/Exchange rate.xlsx
+++ b/Exchange rate.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="36">
   <si>
     <t>TABLE</t>
   </si>
@@ -45,24 +45,6 @@
     <t>mid</t>
   </si>
   <si>
-    <t>040/A/NBP/2021</t>
-  </si>
-  <si>
-    <t>2021-03-01</t>
-  </si>
-  <si>
-    <t>4.5231</t>
-  </si>
-  <si>
-    <t>041/A/NBP/2021</t>
-  </si>
-  <si>
-    <t>2021-03-02</t>
-  </si>
-  <si>
-    <t>4.5345</t>
-  </si>
-  <si>
     <t>042/A/NBP/2021</t>
   </si>
   <si>
@@ -90,19 +72,55 @@
     <t>4.5793</t>
   </si>
   <si>
+    <t>045/A/NBP/2021</t>
+  </si>
+  <si>
+    <t>2021-03-08</t>
+  </si>
+  <si>
+    <t>4.5903</t>
+  </si>
+  <si>
+    <t>046/A/NBP/2021</t>
+  </si>
+  <si>
+    <t>2021-03-09</t>
+  </si>
+  <si>
+    <t>4.5844</t>
+  </si>
+  <si>
+    <t>047/A/NBP/2021</t>
+  </si>
+  <si>
+    <t>2021-03-10</t>
+  </si>
+  <si>
+    <t>4.5718</t>
+  </si>
+  <si>
     <t>dolar amerykański</t>
   </si>
   <si>
     <t>USD</t>
   </si>
   <si>
-    <t>3.7572</t>
-  </si>
-  <si>
-    <t>3.7765</t>
-  </si>
-  <si>
     <t>3.7509</t>
+  </si>
+  <si>
+    <t>3.7851</t>
+  </si>
+  <si>
+    <t>3.8393</t>
+  </si>
+  <si>
+    <t>3.8665</t>
+  </si>
+  <si>
+    <t>3.8507</t>
+  </si>
+  <si>
+    <t>3.842</t>
   </si>
 </sst>
 </file>
@@ -195,7 +213,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -298,6 +316,17 @@
         <v>24</v>
       </c>
     </row>
+    <row r="8">
+      <c r="D8" t="s" s="3">
+        <v>25</v>
+      </c>
+      <c r="E8" t="s" s="3">
+        <v>26</v>
+      </c>
+      <c r="F8" t="s" s="3">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="D1:F1"/>
@@ -308,7 +337,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -341,10 +370,10 @@
         <v>4</v>
       </c>
       <c r="B2" t="s" s="5">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C2" t="s" s="5">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D2" t="s" s="5">
         <v>7</v>
@@ -364,7 +393,7 @@
         <v>11</v>
       </c>
       <c r="F3" t="s" s="6">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4">
@@ -375,7 +404,7 @@
         <v>14</v>
       </c>
       <c r="F4" t="s" s="6">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5">
@@ -386,7 +415,40 @@
         <v>17</v>
       </c>
       <c r="F5" t="s" s="6">
-        <v>29</v>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="D6" t="s" s="6">
+        <v>19</v>
+      </c>
+      <c r="E6" t="s" s="6">
+        <v>20</v>
+      </c>
+      <c r="F6" t="s" s="6">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="D7" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="E7" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="F7" t="s" s="6">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="D8" t="s" s="6">
+        <v>25</v>
+      </c>
+      <c r="E8" t="s" s="6">
+        <v>26</v>
+      </c>
+      <c r="F8" t="s" s="6">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
App finally ready. Executable JAR to do.
</commit_message>
<xml_diff>
--- a/Exchange rate.xlsx
+++ b/Exchange rate.xlsx
@@ -6,16 +6,16 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="dolar amerykański id 0.93782327" r:id="rId3" sheetId="1"/>
-    <sheet name="euro id 0.760571048889652" r:id="rId4" sheetId="2"/>
-    <sheet name="funt szterling id 0.19381184153" r:id="rId5" sheetId="3"/>
-    <sheet name="yuan renminbi (Chiny) id 0.7477" r:id="rId6" sheetId="4"/>
+    <sheet name="euro id 0.38009425748389225" r:id="rId3" sheetId="1"/>
+    <sheet name="dolar amerykański id 0.92024677" r:id="rId4" sheetId="2"/>
+    <sheet name="funt szterling id 0.40021683445" r:id="rId5" sheetId="3"/>
+    <sheet name="dolar kanadyjski id 0.140940833" r:id="rId6" sheetId="4"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="106">
   <si>
     <t>TABLE</t>
   </si>
@@ -32,181 +32,205 @@
     <t>A</t>
   </si>
   <si>
+    <t>euro</t>
+  </si>
+  <si>
+    <t>EUR</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>effectiveDate</t>
+  </si>
+  <si>
+    <t>mid</t>
+  </si>
+  <si>
+    <t>040/A/NBP/2021</t>
+  </si>
+  <si>
+    <t>2021-03-01</t>
+  </si>
+  <si>
+    <t>4.5231</t>
+  </si>
+  <si>
+    <t>041/A/NBP/2021</t>
+  </si>
+  <si>
+    <t>2021-03-02</t>
+  </si>
+  <si>
+    <t>4.5345</t>
+  </si>
+  <si>
+    <t>042/A/NBP/2021</t>
+  </si>
+  <si>
+    <t>2021-03-03</t>
+  </si>
+  <si>
+    <t>4.5393</t>
+  </si>
+  <si>
+    <t>043/A/NBP/2021</t>
+  </si>
+  <si>
+    <t>2021-03-04</t>
+  </si>
+  <si>
+    <t>4.554</t>
+  </si>
+  <si>
+    <t>044/A/NBP/2021</t>
+  </si>
+  <si>
+    <t>2021-03-05</t>
+  </si>
+  <si>
+    <t>4.5793</t>
+  </si>
+  <si>
+    <t>045/A/NBP/2021</t>
+  </si>
+  <si>
+    <t>2021-03-08</t>
+  </si>
+  <si>
+    <t>4.5903</t>
+  </si>
+  <si>
+    <t>046/A/NBP/2021</t>
+  </si>
+  <si>
+    <t>2021-03-09</t>
+  </si>
+  <si>
+    <t>4.5844</t>
+  </si>
+  <si>
+    <t>047/A/NBP/2021</t>
+  </si>
+  <si>
+    <t>2021-03-10</t>
+  </si>
+  <si>
+    <t>4.5718</t>
+  </si>
+  <si>
+    <t>048/A/NBP/2021</t>
+  </si>
+  <si>
+    <t>2021-03-11</t>
+  </si>
+  <si>
+    <t>4.5805</t>
+  </si>
+  <si>
+    <t>049/A/NBP/2021</t>
+  </si>
+  <si>
+    <t>2021-03-12</t>
+  </si>
+  <si>
+    <t>4.5909</t>
+  </si>
+  <si>
+    <t>050/A/NBP/2021</t>
+  </si>
+  <si>
+    <t>2021-03-15</t>
+  </si>
+  <si>
+    <t>4.5836</t>
+  </si>
+  <si>
+    <t>051/A/NBP/2021</t>
+  </si>
+  <si>
+    <t>2021-03-16</t>
+  </si>
+  <si>
+    <t>4.5949</t>
+  </si>
+  <si>
+    <t>052/A/NBP/2021</t>
+  </si>
+  <si>
+    <t>2021-03-17</t>
+  </si>
+  <si>
+    <t>4.6065</t>
+  </si>
+  <si>
+    <t>053/A/NBP/2021</t>
+  </si>
+  <si>
+    <t>2021-03-18</t>
+  </si>
+  <si>
+    <t>4.6224</t>
+  </si>
+  <si>
+    <t>054/A/NBP/2021</t>
+  </si>
+  <si>
+    <t>2021-03-19</t>
+  </si>
+  <si>
+    <t>4.6226</t>
+  </si>
+  <si>
     <t>dolar amerykański</t>
   </si>
   <si>
     <t>USD</t>
   </si>
   <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>effectiveDate</t>
-  </si>
-  <si>
-    <t>mid</t>
-  </si>
-  <si>
-    <t>040/A/NBP/2021</t>
-  </si>
-  <si>
-    <t>2021-03-01</t>
-  </si>
-  <si>
     <t>3.7572</t>
   </si>
   <si>
-    <t>041/A/NBP/2021</t>
-  </si>
-  <si>
-    <t>2021-03-02</t>
-  </si>
-  <si>
     <t>3.7765</t>
   </si>
   <si>
-    <t>042/A/NBP/2021</t>
-  </si>
-  <si>
-    <t>2021-03-03</t>
-  </si>
-  <si>
     <t>3.7509</t>
   </si>
   <si>
-    <t>043/A/NBP/2021</t>
-  </si>
-  <si>
-    <t>2021-03-04</t>
-  </si>
-  <si>
     <t>3.7851</t>
   </si>
   <si>
-    <t>044/A/NBP/2021</t>
-  </si>
-  <si>
-    <t>2021-03-05</t>
-  </si>
-  <si>
     <t>3.8393</t>
   </si>
   <si>
-    <t>045/A/NBP/2021</t>
-  </si>
-  <si>
-    <t>2021-03-08</t>
-  </si>
-  <si>
     <t>3.8665</t>
   </si>
   <si>
-    <t>046/A/NBP/2021</t>
-  </si>
-  <si>
-    <t>2021-03-09</t>
-  </si>
-  <si>
     <t>3.8507</t>
   </si>
   <si>
-    <t>047/A/NBP/2021</t>
-  </si>
-  <si>
-    <t>2021-03-10</t>
-  </si>
-  <si>
     <t>3.842</t>
   </si>
   <si>
-    <t>048/A/NBP/2021</t>
-  </si>
-  <si>
-    <t>2021-03-11</t>
-  </si>
-  <si>
     <t>3.8287</t>
   </si>
   <si>
-    <t>049/A/NBP/2021</t>
-  </si>
-  <si>
-    <t>2021-03-12</t>
-  </si>
-  <si>
     <t>3.8521</t>
   </si>
   <si>
-    <t>050/A/NBP/2021</t>
-  </si>
-  <si>
-    <t>2021-03-15</t>
-  </si>
-  <si>
     <t>3.8429</t>
   </si>
   <si>
-    <t>051/A/NBP/2021</t>
-  </si>
-  <si>
-    <t>2021-03-16</t>
-  </si>
-  <si>
     <t>3.8519</t>
   </si>
   <si>
-    <t>052/A/NBP/2021</t>
-  </si>
-  <si>
-    <t>2021-03-17</t>
-  </si>
-  <si>
     <t>3.8676</t>
   </si>
   <si>
-    <t>euro</t>
-  </si>
-  <si>
-    <t>EUR</t>
-  </si>
-  <si>
-    <t>4.5231</t>
-  </si>
-  <si>
-    <t>4.5345</t>
-  </si>
-  <si>
-    <t>4.5393</t>
-  </si>
-  <si>
-    <t>4.554</t>
-  </si>
-  <si>
-    <t>4.5793</t>
-  </si>
-  <si>
-    <t>4.5903</t>
-  </si>
-  <si>
-    <t>4.5844</t>
-  </si>
-  <si>
-    <t>4.5718</t>
-  </si>
-  <si>
-    <t>4.5805</t>
-  </si>
-  <si>
-    <t>4.5909</t>
-  </si>
-  <si>
-    <t>4.5836</t>
-  </si>
-  <si>
-    <t>4.5949</t>
-  </si>
-  <si>
-    <t>4.6065</t>
+    <t>3.8705</t>
+  </si>
+  <si>
+    <t>3.8865</t>
   </si>
   <si>
     <t>funt szterling</t>
@@ -254,49 +278,61 @@
     <t>5.3758</t>
   </si>
   <si>
-    <t>yuan renminbi (Chiny)</t>
-  </si>
-  <si>
-    <t>CNY</t>
-  </si>
-  <si>
-    <t>0.5811</t>
-  </si>
-  <si>
-    <t>0.5836</t>
-  </si>
-  <si>
-    <t>0.5803</t>
-  </si>
-  <si>
-    <t>0.585</t>
-  </si>
-  <si>
-    <t>0.5922</t>
-  </si>
-  <si>
-    <t>0.5923</t>
-  </si>
-  <si>
-    <t>0.591</t>
-  </si>
-  <si>
-    <t>0.5904</t>
-  </si>
-  <si>
-    <t>0.5899</t>
-  </si>
-  <si>
-    <t>0.5919</t>
-  </si>
-  <si>
-    <t>0.5913</t>
-  </si>
-  <si>
-    <t>0.5924</t>
-  </si>
-  <si>
-    <t>0.5949</t>
+    <t>5.4038</t>
+  </si>
+  <si>
+    <t>5.4116</t>
+  </si>
+  <si>
+    <t>dolar kanadyjski</t>
+  </si>
+  <si>
+    <t>CAD</t>
+  </si>
+  <si>
+    <t>2.9589</t>
+  </si>
+  <si>
+    <t>2.9803</t>
+  </si>
+  <si>
+    <t>2.9771</t>
+  </si>
+  <si>
+    <t>2.9906</t>
+  </si>
+  <si>
+    <t>3.0231</t>
+  </si>
+  <si>
+    <t>3.0477</t>
+  </si>
+  <si>
+    <t>3.0533</t>
+  </si>
+  <si>
+    <t>3.0374</t>
+  </si>
+  <si>
+    <t>3.0434</t>
+  </si>
+  <si>
+    <t>3.0669</t>
+  </si>
+  <si>
+    <t>3.0861</t>
+  </si>
+  <si>
+    <t>3.0848</t>
+  </si>
+  <si>
+    <t>3.1017</t>
+  </si>
+  <si>
+    <t>3.1206</t>
+  </si>
+  <si>
+    <t>3.1125</t>
   </si>
 </sst>
 </file>
@@ -427,7 +463,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -618,6 +654,28 @@
         <v>48</v>
       </c>
     </row>
+    <row r="16">
+      <c r="D16" t="s" s="3">
+        <v>49</v>
+      </c>
+      <c r="E16" t="s" s="3">
+        <v>50</v>
+      </c>
+      <c r="F16" t="s" s="3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="D17" t="s" s="3">
+        <v>52</v>
+      </c>
+      <c r="E17" t="s" s="3">
+        <v>53</v>
+      </c>
+      <c r="F17" t="s" s="3">
+        <v>54</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="D1:F1"/>
@@ -628,7 +686,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -661,10 +719,10 @@
         <v>4</v>
       </c>
       <c r="B2" t="s" s="5">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="C2" t="s" s="5">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="D2" t="s" s="5">
         <v>7</v>
@@ -684,7 +742,7 @@
         <v>11</v>
       </c>
       <c r="F3" t="s" s="6">
-        <v>51</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4">
@@ -695,7 +753,7 @@
         <v>14</v>
       </c>
       <c r="F4" t="s" s="6">
-        <v>52</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5">
@@ -706,7 +764,7 @@
         <v>17</v>
       </c>
       <c r="F5" t="s" s="6">
-        <v>53</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6">
@@ -717,7 +775,7 @@
         <v>20</v>
       </c>
       <c r="F6" t="s" s="6">
-        <v>54</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7">
@@ -728,7 +786,7 @@
         <v>23</v>
       </c>
       <c r="F7" t="s" s="6">
-        <v>55</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8">
@@ -739,7 +797,7 @@
         <v>26</v>
       </c>
       <c r="F8" t="s" s="6">
-        <v>56</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9">
@@ -750,7 +808,7 @@
         <v>29</v>
       </c>
       <c r="F9" t="s" s="6">
-        <v>57</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10">
@@ -761,7 +819,7 @@
         <v>32</v>
       </c>
       <c r="F10" t="s" s="6">
-        <v>58</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11">
@@ -772,7 +830,7 @@
         <v>35</v>
       </c>
       <c r="F11" t="s" s="6">
-        <v>59</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12">
@@ -783,7 +841,7 @@
         <v>38</v>
       </c>
       <c r="F12" t="s" s="6">
-        <v>60</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13">
@@ -794,7 +852,7 @@
         <v>41</v>
       </c>
       <c r="F13" t="s" s="6">
-        <v>61</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14">
@@ -805,7 +863,7 @@
         <v>44</v>
       </c>
       <c r="F14" t="s" s="6">
-        <v>62</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15">
@@ -816,7 +874,29 @@
         <v>47</v>
       </c>
       <c r="F15" t="s" s="6">
-        <v>63</v>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="D16" t="s" s="6">
+        <v>49</v>
+      </c>
+      <c r="E16" t="s" s="6">
+        <v>50</v>
+      </c>
+      <c r="F16" t="s" s="6">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="D17" t="s" s="6">
+        <v>52</v>
+      </c>
+      <c r="E17" t="s" s="6">
+        <v>53</v>
+      </c>
+      <c r="F17" t="s" s="6">
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -829,7 +909,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -862,10 +942,10 @@
         <v>4</v>
       </c>
       <c r="B2" t="s" s="8">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="C2" t="s" s="8">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="D2" t="s" s="8">
         <v>7</v>
@@ -885,7 +965,7 @@
         <v>11</v>
       </c>
       <c r="F3" t="s" s="9">
-        <v>66</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4">
@@ -896,7 +976,7 @@
         <v>14</v>
       </c>
       <c r="F4" t="s" s="9">
-        <v>67</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5">
@@ -907,7 +987,7 @@
         <v>17</v>
       </c>
       <c r="F5" t="s" s="9">
-        <v>68</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6">
@@ -918,7 +998,7 @@
         <v>20</v>
       </c>
       <c r="F6" t="s" s="9">
-        <v>69</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7">
@@ -929,7 +1009,7 @@
         <v>23</v>
       </c>
       <c r="F7" t="s" s="9">
-        <v>70</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8">
@@ -940,7 +1020,7 @@
         <v>26</v>
       </c>
       <c r="F8" t="s" s="9">
-        <v>71</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9">
@@ -951,7 +1031,7 @@
         <v>29</v>
       </c>
       <c r="F9" t="s" s="9">
-        <v>72</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10">
@@ -962,7 +1042,7 @@
         <v>32</v>
       </c>
       <c r="F10" t="s" s="9">
-        <v>73</v>
+        <v>81</v>
       </c>
     </row>
     <row r="11">
@@ -973,7 +1053,7 @@
         <v>35</v>
       </c>
       <c r="F11" t="s" s="9">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="12">
@@ -984,7 +1064,7 @@
         <v>38</v>
       </c>
       <c r="F12" t="s" s="9">
-        <v>75</v>
+        <v>83</v>
       </c>
     </row>
     <row r="13">
@@ -995,7 +1075,7 @@
         <v>41</v>
       </c>
       <c r="F13" t="s" s="9">
-        <v>76</v>
+        <v>84</v>
       </c>
     </row>
     <row r="14">
@@ -1006,7 +1086,7 @@
         <v>44</v>
       </c>
       <c r="F14" t="s" s="9">
-        <v>77</v>
+        <v>85</v>
       </c>
     </row>
     <row r="15">
@@ -1017,7 +1097,29 @@
         <v>47</v>
       </c>
       <c r="F15" t="s" s="9">
-        <v>78</v>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="D16" t="s" s="9">
+        <v>49</v>
+      </c>
+      <c r="E16" t="s" s="9">
+        <v>50</v>
+      </c>
+      <c r="F16" t="s" s="9">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="D17" t="s" s="9">
+        <v>52</v>
+      </c>
+      <c r="E17" t="s" s="9">
+        <v>53</v>
+      </c>
+      <c r="F17" t="s" s="9">
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -1030,7 +1132,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1063,10 +1165,10 @@
         <v>4</v>
       </c>
       <c r="B2" t="s" s="11">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="C2" t="s" s="11">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="D2" t="s" s="11">
         <v>7</v>
@@ -1086,7 +1188,7 @@
         <v>11</v>
       </c>
       <c r="F3" t="s" s="12">
-        <v>81</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4">
@@ -1097,7 +1199,7 @@
         <v>14</v>
       </c>
       <c r="F4" t="s" s="12">
-        <v>82</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5">
@@ -1108,7 +1210,7 @@
         <v>17</v>
       </c>
       <c r="F5" t="s" s="12">
-        <v>83</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6">
@@ -1119,7 +1221,7 @@
         <v>20</v>
       </c>
       <c r="F6" t="s" s="12">
-        <v>84</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7">
@@ -1130,7 +1232,7 @@
         <v>23</v>
       </c>
       <c r="F7" t="s" s="12">
-        <v>85</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8">
@@ -1141,7 +1243,7 @@
         <v>26</v>
       </c>
       <c r="F8" t="s" s="12">
-        <v>86</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9">
@@ -1152,7 +1254,7 @@
         <v>29</v>
       </c>
       <c r="F9" t="s" s="12">
-        <v>87</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10">
@@ -1163,7 +1265,7 @@
         <v>32</v>
       </c>
       <c r="F10" t="s" s="12">
-        <v>88</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11">
@@ -1174,7 +1276,7 @@
         <v>35</v>
       </c>
       <c r="F11" t="s" s="12">
-        <v>89</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12">
@@ -1185,7 +1287,7 @@
         <v>38</v>
       </c>
       <c r="F12" t="s" s="12">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13">
@@ -1196,7 +1298,7 @@
         <v>41</v>
       </c>
       <c r="F13" t="s" s="12">
-        <v>91</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14">
@@ -1207,7 +1309,7 @@
         <v>44</v>
       </c>
       <c r="F14" t="s" s="12">
-        <v>92</v>
+        <v>102</v>
       </c>
     </row>
     <row r="15">
@@ -1218,7 +1320,29 @@
         <v>47</v>
       </c>
       <c r="F15" t="s" s="12">
-        <v>93</v>
+        <v>103</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="D16" t="s" s="12">
+        <v>49</v>
+      </c>
+      <c r="E16" t="s" s="12">
+        <v>50</v>
+      </c>
+      <c r="F16" t="s" s="12">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="D17" t="s" s="12">
+        <v>52</v>
+      </c>
+      <c r="E17" t="s" s="12">
+        <v>53</v>
+      </c>
+      <c r="F17" t="s" s="12">
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
App finally ready. Executable JAR work.
</commit_message>
<xml_diff>
--- a/Exchange rate.xlsx
+++ b/Exchange rate.xlsx
@@ -6,16 +6,16 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="euro id 0.4509753114126611" r:id="rId3" sheetId="1"/>
-    <sheet name="dolar amerykański id 0.91882576" r:id="rId4" sheetId="2"/>
-    <sheet name="funt szterling id 0.00672043008" r:id="rId5" sheetId="3"/>
-    <sheet name="dolar kanadyjski id 0.461727460" r:id="rId6" sheetId="4"/>
+    <sheet name="euro id 0.46256081139439476" r:id="rId3" sheetId="1"/>
+    <sheet name="dolar kanadyjski id 0.395728531" r:id="rId4" sheetId="2"/>
+    <sheet name="funt szterling id 0.59314708960" r:id="rId5" sheetId="3"/>
+    <sheet name="jen (Japonia) id 0.863172385910" r:id="rId6" sheetId="4"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="58">
   <si>
     <t>TABLE</t>
   </si>
@@ -47,6 +47,51 @@
     <t>mid</t>
   </si>
   <si>
+    <t>079/A/NBP/2021</t>
+  </si>
+  <si>
+    <t>2021-04-26</t>
+  </si>
+  <si>
+    <t>4.5565</t>
+  </si>
+  <si>
+    <t>080/A/NBP/2021</t>
+  </si>
+  <si>
+    <t>2021-04-27</t>
+  </si>
+  <si>
+    <t>4.5613</t>
+  </si>
+  <si>
+    <t>081/A/NBP/2021</t>
+  </si>
+  <si>
+    <t>2021-04-28</t>
+  </si>
+  <si>
+    <t>4.5811</t>
+  </si>
+  <si>
+    <t>082/A/NBP/2021</t>
+  </si>
+  <si>
+    <t>2021-04-29</t>
+  </si>
+  <si>
+    <t>4.5782</t>
+  </si>
+  <si>
+    <t>083/A/NBP/2021</t>
+  </si>
+  <si>
+    <t>2021-04-30</t>
+  </si>
+  <si>
+    <t>4.5654</t>
+  </si>
+  <si>
     <t>084/A/NBP/2021</t>
   </si>
   <si>
@@ -65,28 +110,31 @@
     <t>4.5752</t>
   </si>
   <si>
-    <t>086/A/NBP/2021</t>
-  </si>
-  <si>
-    <t>2021-05-06</t>
-  </si>
-  <si>
-    <t>4.5829</t>
-  </si>
-  <si>
-    <t>dolar amerykański</t>
-  </si>
-  <si>
-    <t>USD</t>
-  </si>
-  <si>
-    <t>3.794</t>
-  </si>
-  <si>
-    <t>3.8136</t>
-  </si>
-  <si>
-    <t>3.8066</t>
+    <t>dolar kanadyjski</t>
+  </si>
+  <si>
+    <t>CAD</t>
+  </si>
+  <si>
+    <t>3.0219</t>
+  </si>
+  <si>
+    <t>3.0467</t>
+  </si>
+  <si>
+    <t>3.0586</t>
+  </si>
+  <si>
+    <t>3.0707</t>
+  </si>
+  <si>
+    <t>3.0749</t>
+  </si>
+  <si>
+    <t>3.0802</t>
+  </si>
+  <si>
+    <t>3.1049</t>
   </si>
   <si>
     <t>funt szterling</t>
@@ -95,28 +143,52 @@
     <t>GBP</t>
   </si>
   <si>
+    <t>5.2359</t>
+  </si>
+  <si>
+    <t>5.2426</t>
+  </si>
+  <si>
+    <t>5.2662</t>
+  </si>
+  <si>
+    <t>5.2681</t>
+  </si>
+  <si>
+    <t>5.2491</t>
+  </si>
+  <si>
     <t>5.2622</t>
   </si>
   <si>
     <t>5.2984</t>
   </si>
   <si>
-    <t>5.2908</t>
-  </si>
-  <si>
-    <t>dolar kanadyjski</t>
-  </si>
-  <si>
-    <t>CAD</t>
-  </si>
-  <si>
-    <t>3.0802</t>
-  </si>
-  <si>
-    <t>3.1049</t>
-  </si>
-  <si>
-    <t>3.1061</t>
+    <t>jen (Japonia)</t>
+  </si>
+  <si>
+    <t>JPY</t>
+  </si>
+  <si>
+    <t>0.034961</t>
+  </si>
+  <si>
+    <t>0.03491</t>
+  </si>
+  <si>
+    <t>0.034829</t>
+  </si>
+  <si>
+    <t>0.034674</t>
+  </si>
+  <si>
+    <t>0.034657</t>
+  </si>
+  <si>
+    <t>0.034673</t>
+  </si>
+  <si>
+    <t>0.034872</t>
   </si>
 </sst>
 </file>
@@ -247,7 +319,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -328,6 +400,50 @@
         <v>18</v>
       </c>
     </row>
+    <row r="6">
+      <c r="D6" t="s" s="3">
+        <v>19</v>
+      </c>
+      <c r="E6" t="s" s="3">
+        <v>20</v>
+      </c>
+      <c r="F6" t="s" s="3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="D7" t="s" s="3">
+        <v>22</v>
+      </c>
+      <c r="E7" t="s" s="3">
+        <v>23</v>
+      </c>
+      <c r="F7" t="s" s="3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="D8" t="s" s="3">
+        <v>25</v>
+      </c>
+      <c r="E8" t="s" s="3">
+        <v>26</v>
+      </c>
+      <c r="F8" t="s" s="3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="D9" t="s" s="3">
+        <v>28</v>
+      </c>
+      <c r="E9" t="s" s="3">
+        <v>29</v>
+      </c>
+      <c r="F9" t="s" s="3">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="D1:F1"/>
@@ -338,7 +454,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -371,10 +487,10 @@
         <v>4</v>
       </c>
       <c r="B2" t="s" s="5">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="C2" t="s" s="5">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="D2" t="s" s="5">
         <v>7</v>
@@ -394,7 +510,7 @@
         <v>11</v>
       </c>
       <c r="F3" t="s" s="6">
-        <v>21</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4">
@@ -405,7 +521,7 @@
         <v>14</v>
       </c>
       <c r="F4" t="s" s="6">
-        <v>22</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5">
@@ -416,7 +532,51 @@
         <v>17</v>
       </c>
       <c r="F5" t="s" s="6">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="D6" t="s" s="6">
+        <v>19</v>
+      </c>
+      <c r="E6" t="s" s="6">
+        <v>20</v>
+      </c>
+      <c r="F6" t="s" s="6">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="D7" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="E7" t="s" s="6">
         <v>23</v>
+      </c>
+      <c r="F7" t="s" s="6">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="D8" t="s" s="6">
+        <v>25</v>
+      </c>
+      <c r="E8" t="s" s="6">
+        <v>26</v>
+      </c>
+      <c r="F8" t="s" s="6">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="D9" t="s" s="6">
+        <v>28</v>
+      </c>
+      <c r="E9" t="s" s="6">
+        <v>29</v>
+      </c>
+      <c r="F9" t="s" s="6">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -429,7 +589,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -462,10 +622,10 @@
         <v>4</v>
       </c>
       <c r="B2" t="s" s="8">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="C2" t="s" s="8">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="D2" t="s" s="8">
         <v>7</v>
@@ -485,7 +645,7 @@
         <v>11</v>
       </c>
       <c r="F3" t="s" s="9">
-        <v>26</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4">
@@ -496,7 +656,7 @@
         <v>14</v>
       </c>
       <c r="F4" t="s" s="9">
-        <v>27</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5">
@@ -507,7 +667,51 @@
         <v>17</v>
       </c>
       <c r="F5" t="s" s="9">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="D6" t="s" s="9">
+        <v>19</v>
+      </c>
+      <c r="E6" t="s" s="9">
+        <v>20</v>
+      </c>
+      <c r="F6" t="s" s="9">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="D7" t="s" s="9">
+        <v>22</v>
+      </c>
+      <c r="E7" t="s" s="9">
+        <v>23</v>
+      </c>
+      <c r="F7" t="s" s="9">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="D8" t="s" s="9">
+        <v>25</v>
+      </c>
+      <c r="E8" t="s" s="9">
+        <v>26</v>
+      </c>
+      <c r="F8" t="s" s="9">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="D9" t="s" s="9">
         <v>28</v>
+      </c>
+      <c r="E9" t="s" s="9">
+        <v>29</v>
+      </c>
+      <c r="F9" t="s" s="9">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -520,7 +724,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -553,10 +757,10 @@
         <v>4</v>
       </c>
       <c r="B2" t="s" s="11">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="C2" t="s" s="11">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="D2" t="s" s="11">
         <v>7</v>
@@ -576,7 +780,7 @@
         <v>11</v>
       </c>
       <c r="F3" t="s" s="12">
-        <v>31</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4">
@@ -587,7 +791,7 @@
         <v>14</v>
       </c>
       <c r="F4" t="s" s="12">
-        <v>32</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5">
@@ -598,7 +802,51 @@
         <v>17</v>
       </c>
       <c r="F5" t="s" s="12">
-        <v>33</v>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="D6" t="s" s="12">
+        <v>19</v>
+      </c>
+      <c r="E6" t="s" s="12">
+        <v>20</v>
+      </c>
+      <c r="F6" t="s" s="12">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="D7" t="s" s="12">
+        <v>22</v>
+      </c>
+      <c r="E7" t="s" s="12">
+        <v>23</v>
+      </c>
+      <c r="F7" t="s" s="12">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="D8" t="s" s="12">
+        <v>25</v>
+      </c>
+      <c r="E8" t="s" s="12">
+        <v>26</v>
+      </c>
+      <c r="F8" t="s" s="12">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="D9" t="s" s="12">
+        <v>28</v>
+      </c>
+      <c r="E9" t="s" s="12">
+        <v>29</v>
+      </c>
+      <c r="F9" t="s" s="12">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>